<commit_message>
Fixing serial numbers and DA45 support
For Spokes Wrapper 3.0 and Spokes EZ Demo (2.8 and 3.0)
</commit_message>
<xml_diff>
--- a/wrappers/DeviceCapabilities.xlsx
+++ b/wrappers/DeviceCapabilities.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="111">
   <si>
     <t>#Spokes Wrapper Device Capabilities List</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>HasMobCallerId</t>
+  </si>
+  <si>
+    <t>AA05</t>
   </si>
 </sst>
 </file>
@@ -714,9 +717,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -868,7 +873,7 @@
         <v>107</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3914,6 +3919,35 @@
       </c>
       <c r="I111" s="4" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G112" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H112" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I112" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>